<commit_message>
Create a blade layout
</commit_message>
<xml_diff>
--- a/database/presidentes3.xlsx
+++ b/database/presidentes3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="774">
   <si>
     <t>Tratamento</t>
   </si>
@@ -2328,6 +2328,15 @@
   </si>
   <si>
     <t>Arquivo</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Google +</t>
   </si>
 </sst>
 </file>
@@ -2726,10 +2735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="58" zoomScaleSheetLayoutView="24" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="58" zoomScaleSheetLayoutView="24" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2742,10 +2751,10 @@
     <col min="8" max="8" width="19.5703125" customWidth="1"/>
     <col min="9" max="9" width="4.85546875" customWidth="1"/>
     <col min="10" max="10" width="25.85546875" customWidth="1"/>
-    <col min="11" max="11" width="25.42578125" customWidth="1"/>
+    <col min="11" max="11" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.5" customHeight="1">
+    <row r="1" spans="1:14" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2779,8 +2788,17 @@
       <c r="K1" s="4" t="s">
         <v>770</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="13.5" customHeight="1">
+      <c r="L1" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>772</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="13.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -2815,7 +2833,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.5" customHeight="1">
+    <row r="3" spans="1:14" ht="13.5" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -2850,7 +2868,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.5" customHeight="1">
+    <row r="4" spans="1:14" ht="13.5" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2885,7 +2903,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="13.5" customHeight="1">
+    <row r="5" spans="1:14" ht="13.5" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -2920,7 +2938,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="13.5" customHeight="1">
+    <row r="6" spans="1:14" ht="13.5" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -2955,7 +2973,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="13.5" customHeight="1">
+    <row r="7" spans="1:14" ht="13.5" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>405</v>
       </c>
@@ -2990,7 +3008,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="13.5" customHeight="1">
+    <row r="8" spans="1:14" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -3025,7 +3043,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="13.5" customHeight="1">
+    <row r="9" spans="1:14" ht="13.5" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -3060,7 +3078,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="13.5" customHeight="1">
+    <row r="10" spans="1:14" ht="13.5" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -3095,7 +3113,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="13.5" customHeight="1">
+    <row r="11" spans="1:14" ht="13.5" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -3130,7 +3148,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="13.5" customHeight="1">
+    <row r="12" spans="1:14" ht="13.5" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -3165,7 +3183,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="13.5" customHeight="1">
+    <row r="13" spans="1:14" ht="13.5" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -3200,7 +3218,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="13.5" customHeight="1">
+    <row r="14" spans="1:14" ht="13.5" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -3235,7 +3253,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="13.5" customHeight="1">
+    <row r="15" spans="1:14" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -3270,7 +3288,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="13.5" customHeight="1">
+    <row r="16" spans="1:14" ht="13.5" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>